<commit_message>
Added comments to variables
</commit_message>
<xml_diff>
--- a/ames_house_prices/documentation/variable_description.xlsx
+++ b/ames_house_prices/documentation/variable_description.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Documents\GitHub\udacity\ames_house_prices\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\udacity\ames_house_prices\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="170">
   <si>
     <t>Description</t>
   </si>
@@ -843,6 +843,21 @@
        Family Sale between family members
        Partial Home was not completed when last assessed (associated with New Homes)
 </t>
+  </si>
+  <si>
+    <t>Type of house</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -1210,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1251,6 +1266,12 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1259,6 +1280,9 @@
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1267,6 +1291,9 @@
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1275,6 +1302,9 @@
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1283,6 +1313,9 @@
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1291,6 +1324,9 @@
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1299,6 +1335,9 @@
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1307,6 +1346,9 @@
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1315,6 +1357,9 @@
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1323,6 +1368,9 @@
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1331,6 +1379,9 @@
       <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1339,6 +1390,9 @@
       <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1347,6 +1401,9 @@
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1355,6 +1412,9 @@
       <c r="D15" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1363,517 +1423,712 @@
       <c r="D16" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="189" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="189" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="189" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="189" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="126" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="299.25" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="299.25" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="126" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="126" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="126" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="E39" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="126" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E42" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>91</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E53" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>111</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="E55" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>117</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="E57" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="E60" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>125</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>127</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>129</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="E63" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="126" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>131</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="E64" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="126" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>133</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="E65" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>135</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>141</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E72" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>149</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="E73" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="E74" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="126" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>155</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>157</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>159</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="189" x14ac:dyDescent="0.25">
+      <c r="E78" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="189" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>161</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="E79" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>163</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>164</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
analysis of target in progress
</commit_message>
<xml_diff>
--- a/ames_house_prices/documentation/variable_description.xlsx
+++ b/ames_house_prices/documentation/variable_description.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$82</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="172">
   <si>
     <t>Description</t>
   </si>
@@ -858,6 +858,12 @@
   </si>
   <si>
     <t>high</t>
+  </si>
+  <si>
+    <t>Numerical</t>
+  </si>
+  <si>
+    <t>Categorical</t>
   </si>
 </sst>
 </file>
@@ -1223,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1263,6 +1269,9 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1277,6 +1286,9 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1288,6 +1300,9 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1299,6 +1314,9 @@
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1310,6 +1328,9 @@
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B6" t="s">
+        <v>170</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1321,6 +1342,9 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B7" t="s">
+        <v>171</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1332,6 +1356,9 @@
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1343,6 +1370,9 @@
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B9" t="s">
+        <v>171</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1354,6 +1384,9 @@
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B10" t="s">
+        <v>171</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1365,6 +1398,9 @@
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B11" t="s">
+        <v>171</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1376,6 +1412,9 @@
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B12" t="s">
+        <v>171</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1387,6 +1426,9 @@
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1398,6 +1440,9 @@
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1409,6 +1454,9 @@
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1420,6 +1468,9 @@
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="B16" t="s">
+        <v>171</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>36</v>
       </c>
@@ -1431,6 +1482,9 @@
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="B17" t="s">
+        <v>171</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1442,6 +1496,9 @@
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
@@ -1453,6 +1510,9 @@
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="B19" t="s">
+        <v>170</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1464,6 +1524,9 @@
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>44</v>
       </c>
@@ -1475,6 +1538,9 @@
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="B21" t="s">
+        <v>170</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1486,6 +1552,9 @@
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="B22" t="s">
+        <v>170</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>48</v>
       </c>
@@ -1497,6 +1566,9 @@
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="B23" t="s">
+        <v>171</v>
+      </c>
       <c r="D23" s="1" t="s">
         <v>50</v>
       </c>
@@ -1508,6 +1580,9 @@
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
       <c r="D24" s="1" t="s">
         <v>52</v>
       </c>
@@ -1519,6 +1594,9 @@
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="B25" t="s">
+        <v>171</v>
+      </c>
       <c r="D25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1530,6 +1608,9 @@
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="B26" t="s">
+        <v>171</v>
+      </c>
       <c r="D26" s="1" t="s">
         <v>56</v>
       </c>
@@ -1541,6 +1622,9 @@
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="B27" t="s">
+        <v>171</v>
+      </c>
       <c r="D27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1552,6 +1636,9 @@
       <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="B28" t="s">
+        <v>170</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>60</v>
       </c>
@@ -1563,6 +1650,9 @@
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="B29" t="s">
+        <v>171</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>62</v>
       </c>
@@ -1574,6 +1664,9 @@
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="B30" t="s">
+        <v>171</v>
+      </c>
       <c r="D30" s="1" t="s">
         <v>64</v>
       </c>
@@ -1585,6 +1678,9 @@
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
       <c r="D31" s="1" t="s">
         <v>66</v>
       </c>
@@ -1596,6 +1692,9 @@
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="B32" t="s">
+        <v>171</v>
+      </c>
       <c r="D32" s="1" t="s">
         <v>68</v>
       </c>
@@ -1607,6 +1706,9 @@
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="B33" t="s">
+        <v>171</v>
+      </c>
       <c r="D33" s="1" t="s">
         <v>70</v>
       </c>
@@ -1618,6 +1720,9 @@
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="B34" t="s">
+        <v>171</v>
+      </c>
       <c r="D34" s="1" t="s">
         <v>72</v>
       </c>
@@ -1629,6 +1734,9 @@
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="B35" t="s">
+        <v>171</v>
+      </c>
       <c r="D35" s="1" t="s">
         <v>74</v>
       </c>
@@ -1640,6 +1748,9 @@
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="B36" t="s">
+        <v>170</v>
+      </c>
       <c r="D36" s="1" t="s">
         <v>76</v>
       </c>
@@ -1651,6 +1762,9 @@
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="B37" t="s">
+        <v>171</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>78</v>
       </c>
@@ -1662,6 +1776,9 @@
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="B38" t="s">
+        <v>170</v>
+      </c>
       <c r="D38" s="1" t="s">
         <v>80</v>
       </c>
@@ -1673,6 +1790,9 @@
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="B39" t="s">
+        <v>170</v>
+      </c>
       <c r="D39" s="1" t="s">
         <v>82</v>
       </c>
@@ -1684,6 +1804,9 @@
       <c r="A40" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="B40" t="s">
+        <v>170</v>
+      </c>
       <c r="D40" s="1" t="s">
         <v>84</v>
       </c>
@@ -1695,6 +1818,9 @@
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="B41" t="s">
+        <v>171</v>
+      </c>
       <c r="D41" s="1" t="s">
         <v>86</v>
       </c>
@@ -1706,6 +1832,9 @@
       <c r="A42" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="B42" t="s">
+        <v>171</v>
+      </c>
       <c r="D42" s="1" t="s">
         <v>88</v>
       </c>
@@ -1717,6 +1846,9 @@
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="B43" t="s">
+        <v>171</v>
+      </c>
       <c r="D43" s="1" t="s">
         <v>90</v>
       </c>
@@ -1728,6 +1860,9 @@
       <c r="A44" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="B44" t="s">
+        <v>171</v>
+      </c>
       <c r="D44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1739,6 +1874,9 @@
       <c r="A45" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="B45" t="s">
+        <v>170</v>
+      </c>
       <c r="D45" s="1" t="s">
         <v>94</v>
       </c>
@@ -1750,6 +1888,9 @@
       <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="B46" t="s">
+        <v>170</v>
+      </c>
       <c r="D46" s="1" t="s">
         <v>96</v>
       </c>
@@ -1761,6 +1902,9 @@
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="B47" t="s">
+        <v>170</v>
+      </c>
       <c r="D47" s="1" t="s">
         <v>98</v>
       </c>
@@ -1772,6 +1916,9 @@
       <c r="A48" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="B48" t="s">
+        <v>170</v>
+      </c>
       <c r="D48" s="1" t="s">
         <v>100</v>
       </c>
@@ -1783,6 +1930,9 @@
       <c r="A49" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="B49" t="s">
+        <v>170</v>
+      </c>
       <c r="D49" s="1" t="s">
         <v>102</v>
       </c>
@@ -1794,6 +1944,9 @@
       <c r="A50" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="B50" t="s">
+        <v>170</v>
+      </c>
       <c r="D50" s="1" t="s">
         <v>104</v>
       </c>
@@ -1805,6 +1958,9 @@
       <c r="A51" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="B51" t="s">
+        <v>170</v>
+      </c>
       <c r="D51" s="1" t="s">
         <v>106</v>
       </c>
@@ -1816,6 +1972,9 @@
       <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="B52" t="s">
+        <v>170</v>
+      </c>
       <c r="D52" s="1" t="s">
         <v>108</v>
       </c>
@@ -1827,6 +1986,9 @@
       <c r="A53" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="B53" t="s">
+        <v>170</v>
+      </c>
       <c r="D53" s="1" t="s">
         <v>110</v>
       </c>
@@ -1838,6 +2000,9 @@
       <c r="A54" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="B54" t="s">
+        <v>170</v>
+      </c>
       <c r="D54" s="1" t="s">
         <v>112</v>
       </c>
@@ -1849,6 +2014,9 @@
       <c r="A55" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="B55" t="s">
+        <v>171</v>
+      </c>
       <c r="D55" s="1" t="s">
         <v>114</v>
       </c>
@@ -1860,6 +2028,9 @@
       <c r="A56" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="B56" t="s">
+        <v>170</v>
+      </c>
       <c r="D56" s="1" t="s">
         <v>116</v>
       </c>
@@ -1871,6 +2042,9 @@
       <c r="A57" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="B57" t="s">
+        <v>171</v>
+      </c>
       <c r="D57" s="1" t="s">
         <v>118</v>
       </c>
@@ -1882,6 +2056,9 @@
       <c r="A58" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="B58" t="s">
+        <v>170</v>
+      </c>
       <c r="D58" s="1" t="s">
         <v>120</v>
       </c>
@@ -1893,6 +2070,9 @@
       <c r="A59" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="B59" t="s">
+        <v>171</v>
+      </c>
       <c r="D59" s="1" t="s">
         <v>122</v>
       </c>
@@ -1904,6 +2084,9 @@
       <c r="A60" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="B60" t="s">
+        <v>171</v>
+      </c>
       <c r="D60" s="1" t="s">
         <v>124</v>
       </c>
@@ -1915,6 +2098,9 @@
       <c r="A61" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="B61" t="s">
+        <v>170</v>
+      </c>
       <c r="D61" s="1" t="s">
         <v>126</v>
       </c>
@@ -1926,6 +2112,9 @@
       <c r="A62" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="B62" t="s">
+        <v>171</v>
+      </c>
       <c r="D62" s="1" t="s">
         <v>128</v>
       </c>
@@ -1937,6 +2126,9 @@
       <c r="A63" s="1" t="s">
         <v>129</v>
       </c>
+      <c r="B63" t="s">
+        <v>170</v>
+      </c>
       <c r="D63" s="1" t="s">
         <v>130</v>
       </c>
@@ -1948,6 +2140,9 @@
       <c r="A64" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="B64" t="s">
+        <v>170</v>
+      </c>
       <c r="D64" s="1" t="s">
         <v>132</v>
       </c>
@@ -1959,6 +2154,9 @@
       <c r="A65" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="B65" t="s">
+        <v>171</v>
+      </c>
       <c r="D65" s="1" t="s">
         <v>134</v>
       </c>
@@ -1970,6 +2168,9 @@
       <c r="A66" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="B66" t="s">
+        <v>171</v>
+      </c>
       <c r="D66" s="1" t="s">
         <v>136</v>
       </c>
@@ -1981,6 +2182,9 @@
       <c r="A67" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="B67" t="s">
+        <v>171</v>
+      </c>
       <c r="D67" s="1" t="s">
         <v>138</v>
       </c>
@@ -1992,6 +2196,9 @@
       <c r="A68" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="B68" t="s">
+        <v>170</v>
+      </c>
       <c r="D68" s="1" t="s">
         <v>140</v>
       </c>
@@ -2003,6 +2210,9 @@
       <c r="A69" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="B69" t="s">
+        <v>170</v>
+      </c>
       <c r="D69" s="1" t="s">
         <v>142</v>
       </c>
@@ -2014,6 +2224,9 @@
       <c r="A70" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="B70" t="s">
+        <v>170</v>
+      </c>
       <c r="D70" s="1" t="s">
         <v>144</v>
       </c>
@@ -2025,6 +2238,9 @@
       <c r="A71" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="B71" t="s">
+        <v>170</v>
+      </c>
       <c r="D71" s="1" t="s">
         <v>146</v>
       </c>
@@ -2036,6 +2252,9 @@
       <c r="A72" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="B72" t="s">
+        <v>170</v>
+      </c>
       <c r="D72" s="1" t="s">
         <v>148</v>
       </c>
@@ -2047,6 +2266,9 @@
       <c r="A73" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="B73" t="s">
+        <v>170</v>
+      </c>
       <c r="D73" s="1" t="s">
         <v>150</v>
       </c>
@@ -2058,6 +2280,9 @@
       <c r="A74" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="B74" t="s">
+        <v>171</v>
+      </c>
       <c r="D74" s="1" t="s">
         <v>152</v>
       </c>
@@ -2069,6 +2294,9 @@
       <c r="A75" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="B75" t="s">
+        <v>171</v>
+      </c>
       <c r="D75" s="1" t="s">
         <v>154</v>
       </c>
@@ -2080,6 +2308,9 @@
       <c r="A76" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="B76" t="s">
+        <v>171</v>
+      </c>
       <c r="D76" s="1" t="s">
         <v>156</v>
       </c>
@@ -2091,6 +2322,9 @@
       <c r="A77" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="B77" t="s">
+        <v>170</v>
+      </c>
       <c r="D77" s="1" t="s">
         <v>158</v>
       </c>
@@ -2102,6 +2336,9 @@
       <c r="A78" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="B78" t="s">
+        <v>170</v>
+      </c>
       <c r="D78" s="1" t="s">
         <v>160</v>
       </c>
@@ -2113,6 +2350,9 @@
       <c r="A79" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="B79" t="s">
+        <v>170</v>
+      </c>
       <c r="D79" s="1" t="s">
         <v>162</v>
       </c>
@@ -2124,6 +2364,9 @@
       <c r="A80" s="1" t="s">
         <v>163</v>
       </c>
+      <c r="B80" t="s">
+        <v>171</v>
+      </c>
       <c r="D80" s="1" t="s">
         <v>164</v>
       </c>
@@ -2131,8 +2374,18 @@
         <v>167</v>
       </c>
     </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G2"/>
+  <autoFilter ref="A1:G82"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
documentation updated and analysis evolution
</commit_message>
<xml_diff>
--- a/ames_house_prices/documentation/variable_description.xlsx
+++ b/ames_house_prices/documentation/variable_description.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$82</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="175">
   <si>
     <t>Description</t>
   </si>
@@ -864,6 +864,15 @@
   </si>
   <si>
     <t>Categorical</t>
+  </si>
+  <si>
+    <t>Convert to Categorical</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1229,20 +1238,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="21.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="70.375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="21.875" style="1" customWidth="1"/>
+    <col min="1" max="4" width="21.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="70.375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="21.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1253,19 +1262,22 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="283.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="283.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1273,44 +1285,50 @@
         <v>170</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1318,195 +1336,201 @@
         <v>170</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>171</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>171</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>171</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>171</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>171</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>171</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>171</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>171</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>171</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>171</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="189" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="189" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="189" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="189" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1514,13 +1538,16 @@
         <v>170</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1528,13 +1555,16 @@
         <v>170</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -1542,237 +1572,249 @@
         <v>170</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="126" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B23" t="s">
         <v>171</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="299.25" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B24" t="s">
         <v>171</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="299.25" x14ac:dyDescent="0.25">
+      <c r="F24" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B25" t="s">
         <v>171</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B26" t="s">
         <v>171</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
-      </c>
-      <c r="D28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B29" t="s">
         <v>171</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="126" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B30" t="s">
         <v>171</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="126" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B31" t="s">
         <v>171</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+      <c r="F31" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="126" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B32" t="s">
         <v>171</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B33" t="s">
         <v>171</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="F33" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B34" t="s">
         <v>171</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>170</v>
-      </c>
-      <c r="D36" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -1780,13 +1822,16 @@
         <v>170</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
@@ -1794,83 +1839,89 @@
         <v>170</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="126" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>170</v>
-      </c>
-      <c r="D40" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B41" t="s">
         <v>171</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B42" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B43" t="s">
         <v>171</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>93</v>
       </c>
@@ -1878,13 +1929,16 @@
         <v>170</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
@@ -1892,13 +1946,16 @@
         <v>170</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
@@ -1906,13 +1963,16 @@
         <v>170</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>99</v>
       </c>
@@ -1920,13 +1980,16 @@
         <v>170</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>101</v>
       </c>
@@ -1934,13 +1997,16 @@
         <v>170</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>103</v>
       </c>
@@ -1948,13 +2014,16 @@
         <v>170</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>105</v>
       </c>
@@ -1962,13 +2031,16 @@
         <v>170</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
@@ -1976,13 +2048,16 @@
         <v>170</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>109</v>
       </c>
@@ -1990,139 +2065,154 @@
         <v>170</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="F53" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>170</v>
-      </c>
-      <c r="D54" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>170</v>
-      </c>
-      <c r="D56" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B58" t="s">
-        <v>170</v>
-      </c>
-      <c r="D58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="F58" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B59" t="s">
         <v>171</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B60" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="F60" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B61" t="s">
-        <v>170</v>
-      </c>
-      <c r="D61" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D62" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>129</v>
       </c>
@@ -2130,69 +2220,75 @@
         <v>170</v>
       </c>
       <c r="D63" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="126" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B64" t="s">
-        <v>170</v>
-      </c>
-      <c r="D64" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+      <c r="F64" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="126" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B65" t="s">
         <v>171</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="F65" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B66" t="s">
         <v>171</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B67" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D67" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>139</v>
       </c>
@@ -2200,13 +2296,16 @@
         <v>170</v>
       </c>
       <c r="D68" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>141</v>
       </c>
@@ -2214,13 +2313,16 @@
         <v>170</v>
       </c>
       <c r="D69" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>143</v>
       </c>
@@ -2228,13 +2330,16 @@
         <v>170</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>145</v>
       </c>
@@ -2242,13 +2347,16 @@
         <v>170</v>
       </c>
       <c r="D71" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>147</v>
       </c>
@@ -2256,69 +2364,75 @@
         <v>170</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="F72" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B73" t="s">
-        <v>170</v>
-      </c>
-      <c r="D73" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="F73" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>151</v>
       </c>
       <c r="B74" t="s">
         <v>171</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+      <c r="F74" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="126" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B75" t="s">
         <v>171</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D76" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E76" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>157</v>
       </c>
@@ -2326,13 +2440,16 @@
         <v>170</v>
       </c>
       <c r="D77" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>159</v>
       </c>
@@ -2340,52 +2457,50 @@
         <v>170</v>
       </c>
       <c r="D78" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="189" x14ac:dyDescent="0.25">
+      <c r="F78" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="189" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B79" t="s">
-        <v>170</v>
-      </c>
-      <c r="D79" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="F79" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B80" t="s">
         <v>171</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="E80" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
         <v>170</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G82"/>
+  <autoFilter ref="A1:H82"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>